<commit_message>
update binance exchange limits docs
</commit_message>
<xml_diff>
--- a/exchange_limits/exchange_limits_binance.xlsx
+++ b/exchange_limits/exchange_limits_binance.xlsx
@@ -57,73 +57,73 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>最小订单金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>LTC</t>
+  </si>
+  <si>
+    <t>BCC</t>
+  </si>
+  <si>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t>USDT</t>
+  </si>
+  <si>
+    <t>最小Volume</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小Volume（单位）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小订单金额（单位）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRICE_FILTER: tickSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOT_SIZE: stepSize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOT_SIZE: minQty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIN_NOTIONAL: min_notional</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小Volume变动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小Volume变动（单位）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小价格变化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最小价格变化（单位）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>etc_btc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小订单金额</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t>BTC</t>
-  </si>
-  <si>
-    <t>LTC</t>
-  </si>
-  <si>
-    <t>BCC</t>
-  </si>
-  <si>
-    <t>ETC</t>
-  </si>
-  <si>
-    <t>USDT</t>
-  </si>
-  <si>
-    <t>最小Volume</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小Volume（单位）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小订单金额（单位）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PRICE_FILTER: tickSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOT_SIZE: stepSize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOT_SIZE: minQty</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MIN_NOTIONAL: min_notional</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小Volume变动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小Volume变动（单位）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小价格变化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>最小价格变化（单位）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,7 +480,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -498,105 +498,129 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>27</v>
-      </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>0.01</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10</v>
+      </c>
       <c r="I3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>0.01</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10</v>
+      </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>0.01</v>
+      </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10</v>
+      </c>
       <c r="I5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -605,82 +629,106 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1E-4</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.01</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.01</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
       <c r="I7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.01</v>
+      </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.01</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.01</v>
+      </c>
       <c r="I8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>0.01</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="I9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -689,61 +737,77 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="I11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B12" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.01</v>
+      </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.01</v>
+      </c>
       <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="I12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bch=bcc, add binance exchange limits of bch
</commit_message>
<xml_diff>
--- a/exchange_limits/exchange_limits_binance.xlsx
+++ b/exchange_limits/exchange_limits_binance.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="binance" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -480,7 +480,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -627,19 +627,27 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>0.01</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>10</v>
+      </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
@@ -735,19 +743,27 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>1E-3</v>
+      </c>
       <c r="I10" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
add eos pairs to binance coinmex
</commit_message>
<xml_diff>
--- a/exchange_limits/exchange_limits_binance.xlsx
+++ b/exchange_limits/exchange_limits_binance.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
   <si>
     <t>btc_usdt</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -124,6 +124,32 @@
   </si>
   <si>
     <t>etc_btc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>eos_eth</t>
+  </si>
+  <si>
+    <t>eos_usdt</t>
+  </si>
+  <si>
+    <t>ETH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USDT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EOS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ETH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -477,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
@@ -492,8 +518,11 @@
     <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
     <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -824,6 +853,64 @@
       </c>
       <c r="I12" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13">
+        <v>0.01</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13">
+        <v>0.01</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13">
+        <v>0.01</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14">
+        <v>1E-4</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14">
+        <v>0.01</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>